<commit_message>
Feature : ItemType enum 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/ConsumalbeDB_Sheet.xlsx
+++ b/Assets/Excel/Items/ConsumalbeDB_Sheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{36698364-F62F-42F9-9B78-296C98B392F1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F96F3EC-A88D-4D72-906E-329FDC94619D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView minimized="1" xWindow="495" yWindow="780" windowWidth="28800" windowHeight="15345" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
   <si>
     <t>_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -82,6 +82,26 @@
   </si>
   <si>
     <t>회복약</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Consumable/Potion_1</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Power Potion</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>공격력 증가</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Items/Icons/Consumable/Potion_2</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Normal</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -407,10 +427,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P2"/>
+  <dimension ref="A1:P3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="D2" sqref="D2"/>
+      <selection activeCell="K14" sqref="K14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
@@ -418,10 +438,10 @@
     <col min="1" max="1" width="13.5" customWidth="1"/>
     <col min="2" max="2" width="15.875" customWidth="1"/>
     <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="25.625" customWidth="1"/>
+    <col min="4" max="4" width="31.125" customWidth="1"/>
     <col min="5" max="5" width="10.875" customWidth="1"/>
     <col min="6" max="6" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="34.25" customWidth="1"/>
+    <col min="7" max="7" width="12.75" customWidth="1"/>
     <col min="11" max="11" width="17" customWidth="1"/>
     <col min="12" max="12" width="11.25" customWidth="1"/>
     <col min="14" max="14" width="11.75" customWidth="1"/>
@@ -489,6 +509,89 @@
       <c r="C2" t="s">
         <v>17</v>
       </c>
+      <c r="D2" t="s">
+        <v>18</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
+        <v>1</v>
+      </c>
+      <c r="H2">
+        <v>20</v>
+      </c>
+      <c r="I2" t="s">
+        <v>22</v>
+      </c>
+      <c r="J2">
+        <v>20</v>
+      </c>
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+      <c r="M2">
+        <v>0</v>
+      </c>
+      <c r="N2">
+        <v>0</v>
+      </c>
+      <c r="O2">
+        <v>0</v>
+      </c>
+      <c r="P2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>10301021</v>
+      </c>
+      <c r="B3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C3" t="s">
+        <v>20</v>
+      </c>
+      <c r="D3" t="s">
+        <v>21</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="F3">
+        <v>1</v>
+      </c>
+      <c r="H3">
+        <v>20</v>
+      </c>
+      <c r="I3" t="s">
+        <v>22</v>
+      </c>
+      <c r="J3">
+        <v>0</v>
+      </c>
+      <c r="K3">
+        <v>0</v>
+      </c>
+      <c r="L3">
+        <v>0</v>
+      </c>
+      <c r="M3">
+        <v>0</v>
+      </c>
+      <c r="N3">
+        <v>0</v>
+      </c>
+      <c r="O3">
+        <v>0</v>
+      </c>
+      <c r="P3">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>

</xml_diff>

<commit_message>
Docs : ItemType 추가
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/ConsumalbeDB_Sheet.xlsx
+++ b/Assets/Excel/Items/ConsumalbeDB_Sheet.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F96F3EC-A88D-4D72-906E-329FDC94619D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE07ED0C-2638-49A2-81CC-47360791A1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="27" uniqueCount="25">
   <si>
     <t>_id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -102,6 +102,14 @@
   </si>
   <si>
     <t>Normal</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>_itemType</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>Consumable</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -427,109 +435,112 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:P3"/>
+  <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="K14" sqref="K14"/>
+      <selection activeCell="M10" sqref="M10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="13.5" customWidth="1"/>
-    <col min="2" max="2" width="15.875" customWidth="1"/>
-    <col min="3" max="3" width="16.375" customWidth="1"/>
-    <col min="4" max="4" width="31.125" customWidth="1"/>
-    <col min="5" max="5" width="10.875" customWidth="1"/>
-    <col min="6" max="6" width="11.75" customWidth="1"/>
-    <col min="7" max="7" width="12.75" customWidth="1"/>
-    <col min="11" max="11" width="17" customWidth="1"/>
-    <col min="12" max="12" width="11.25" customWidth="1"/>
-    <col min="14" max="14" width="11.75" customWidth="1"/>
-    <col min="15" max="15" width="12.625" customWidth="1"/>
-    <col min="16" max="16" width="13" customWidth="1"/>
+    <col min="1" max="2" width="13.5" customWidth="1"/>
+    <col min="3" max="3" width="15.875" customWidth="1"/>
+    <col min="4" max="4" width="16.375" customWidth="1"/>
+    <col min="5" max="5" width="31.125" customWidth="1"/>
+    <col min="6" max="6" width="10.875" customWidth="1"/>
+    <col min="7" max="7" width="11.75" customWidth="1"/>
+    <col min="8" max="8" width="12.75" customWidth="1"/>
+    <col min="12" max="12" width="17" customWidth="1"/>
+    <col min="13" max="13" width="11.25" customWidth="1"/>
+    <col min="15" max="15" width="11.75" customWidth="1"/>
+    <col min="16" max="16" width="12.625" customWidth="1"/>
+    <col min="17" max="17" width="13" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
       <c r="B1" t="s">
+        <v>23</v>
+      </c>
+      <c r="C1" t="s">
         <v>1</v>
       </c>
-      <c r="C1" t="s">
+      <c r="D1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="E1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="F1" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="H1" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="I1" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="J1" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="K1" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="L1" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="M1" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="N1" t="s">
         <v>12</v>
       </c>
-      <c r="N1" t="s">
+      <c r="O1" t="s">
         <v>13</v>
       </c>
-      <c r="O1" t="s">
+      <c r="P1" t="s">
         <v>14</v>
       </c>
-      <c r="P1" t="s">
+      <c r="Q1" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>10301011</v>
       </c>
       <c r="B2" t="s">
+        <v>24</v>
+      </c>
+      <c r="C2" t="s">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
+      <c r="D2" t="s">
         <v>17</v>
       </c>
-      <c r="D2" t="s">
+      <c r="E2" t="s">
         <v>18</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
       </c>
       <c r="F2">
         <v>1</v>
       </c>
-      <c r="H2">
+      <c r="G2">
+        <v>1</v>
+      </c>
+      <c r="I2">
         <v>20</v>
       </c>
-      <c r="I2" t="s">
+      <c r="J2" t="s">
         <v>22</v>
       </c>
-      <c r="J2">
+      <c r="K2">
         <v>20</v>
       </c>
-      <c r="K2">
-        <v>0</v>
-      </c>
       <c r="L2">
         <v>0</v>
       </c>
@@ -545,35 +556,38 @@
       <c r="P2">
         <v>0</v>
       </c>
+      <c r="Q2">
+        <v>0</v>
+      </c>
     </row>
-    <row r="3" spans="1:16" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>10301021</v>
       </c>
       <c r="B3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C3" t="s">
         <v>19</v>
       </c>
-      <c r="C3" t="s">
+      <c r="D3" t="s">
         <v>20</v>
       </c>
-      <c r="D3" t="s">
+      <c r="E3" t="s">
         <v>21</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
       </c>
       <c r="F3">
         <v>1</v>
       </c>
-      <c r="H3">
+      <c r="G3">
+        <v>1</v>
+      </c>
+      <c r="I3">
         <v>20</v>
       </c>
-      <c r="I3" t="s">
+      <c r="J3" t="s">
         <v>22</v>
       </c>
-      <c r="J3">
-        <v>0</v>
-      </c>
       <c r="K3">
         <v>0</v>
       </c>
@@ -591,6 +605,9 @@
       </c>
       <c r="P3">
         <v>0</v>
+      </c>
+      <c r="Q3">
+        <v>1</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Docs : Consumable SO 생성
</commit_message>
<xml_diff>
--- a/Assets/Excel/Items/ConsumalbeDB_Sheet.xlsx
+++ b/Assets/Excel/Items/ConsumalbeDB_Sheet.xlsx
@@ -8,12 +8,12 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\babyg\Desktop\Coding\unity\Sisyphus\Assets\Excel\Items\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE07ED0C-2638-49A2-81CC-47360791A1BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E552725A-E357-4C3E-B11F-636D9F2C2EB2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="38280" yWindow="1050" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Entities" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -438,7 +438,7 @@
   <dimension ref="A1:Q3"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <selection activeCell="M10" sqref="M10"/>
+      <selection activeCell="E16" sqref="E16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="16.5" x14ac:dyDescent="0.3"/>

</xml_diff>